<commit_message>
Set using emb model in bertopic to approx thetas
</commit_message>
<xml_diff>
--- a/data/top_docs/mallet/thetas_thr_top_docs.xlsx
+++ b/data/top_docs/mallet/thetas_thr_top_docs.xlsx
@@ -476,23 +476,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['episode', 'mulder', 'doctor', 'scully', 'viewers', 'episodes', 'series', 'television', 'character', 'season', 'watched', 'dwight', 'broadcast', 'trek', 'jack']</t>
+          <t>['album', 'song', 'madonna', 'chart', 'video', 'music', 'band', 'songs', 'harrison', 'carey', 'track', 'pop', 'recording', 'vocals', 'lyrics']</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.6679133720936666</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.6662718018536298</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.6545365919096457</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.59602983585893</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.5094743879575174</v>
       </c>
     </row>
     <row r="3">
@@ -501,23 +501,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['album', 'song', 'madonna', 'chart', 'video', 'music', 'harrison', 'songs', 'carey', 'band', 'pop', 'track', 'recording', 'billboard', 'number']</t>
+          <t>['ship', 'guns', 'ships', 'tons', 'torpedo', 'knots', 'inch', 'cruiser', 'fleet', 'gun', 'deck', 'admiral', 'cruisers', 'turrets', 'german']</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7797157170189593</v>
+        <v>0.8997181592361042</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6961537650392843</v>
+        <v>0.8996268402343696</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6599544747492919</v>
+        <v>0.8996111918219933</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6585169491760476</v>
+        <v>0.8991845710025499</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6467437531982382</v>
+        <v>0.8991325241618346</v>
       </c>
     </row>
     <row r="4">
@@ -526,23 +526,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['ship', 'guns', 'ships', 'tons', 'torpedo', 'knots', 'inch', 'cruiser', 'fleet', 'gun', 'deck', 'admiral', 'german', 'turrets', 'cruisers']</t>
+          <t>['episode', 'mulder', 'scully', 'doctor', 'episodes', 'trek', 'series', 'enterprise', 'character', 'viewers', 'files', 'amy', 'television', 'fringe', 'scene']</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.8995174911302904</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8973708912050163</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8949955454517495</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.894203330176475</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8929476064634039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -551,23 +551,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['highway', 'route', 'road', 'freeway', 'interchange', 'intersection', 'terminus', 'north', 'east', 'lane', 'continues', 'state', 'avenue', 'passes', 'traffic']</t>
+          <t>['game', 'player', 'gameplay', 'games', 'players', 'playstation', 'nintendo', 'released', 'graphics', 'characters', 'soundtrack', 'xbox', 'mode', 'version', 'manga']</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8994529065196937</v>
+        <v>0.5043347996538532</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8979494389191461</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8973824479064191</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8960262822473475</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8913213516555959</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -576,23 +576,23 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['election', 'hitler', 'campaign', 'party', 'bush', 'republican', 'political', 'vote', 'labour', 'president', 'presidential', 'democratic', 'war', 'government', 'senate']</t>
+          <t>['innings', 'team', 'runs', 'match', 'league', 'nba', 'baseball', 'batting', 'season', 'career', 'scored', 'wickets', 'championship', 'cricket', 'basketball']</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.8868632889016513</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.530041659289464</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.5190010126251009</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.515382931222915</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.5051943860553056</v>
       </c>
     </row>
     <row r="7">
@@ -601,23 +601,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['tropical', 'storm', 'hurricane', 'winds', 'depression', 'cyclone', 'mph', 'rainfall', 'damage', 'landfall', 'wind', 'utc', 'flooding', 'weakened', 'intensity']</t>
+          <t>['highway', 'route', 'road', 'freeway', 'interchange', 'intersection', 'terminus', 'north', 'east', 'continues', 'lane', 'state', 'avenue', 'passes', 'crosses']</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.8994931954472305</v>
+        <v>0.899801649477929</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8989416131641279</v>
+        <v>0.8961865609855832</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8983367875255148</v>
+        <v>0.8939007380530359</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8911209008282481</v>
+        <v>0.8921215893160269</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8898994247877255</v>
+        <v>0.8871423952289832</v>
       </c>
     </row>
     <row r="8">
@@ -626,23 +626,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['king', 'government', 'polish', 'political', 'emperor', 'son', 'arab', 'death', 'military', 'army', 'died', 'pope', 'poland', 'reign', 'byzantine']</t>
+          <t>['tropical', 'storm', 'hurricane', 'winds', 'depression', 'cyclone', 'mph', 'rainfall', 'damage', 'landfall', 'utc', 'wind', 'flooding', 'weakened', 'intensity']</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.8992052213768034</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.8984309546456318</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.8924736905627255</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.889391766810613</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.8891288162450154</v>
       </c>
     </row>
     <row r="9">
@@ -651,20 +651,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['species', 'shark', 'genus', 'sharks', 'females', 'prey', 'eggs', 'males', 'cap', 'birds', 'nest', 'habitat', 'fin', 'brown', 'stem']</t>
+          <t>['film', 'films', 'disney', 'movie', 'animated', 'role', 'comedy', 'simpsons', 'starred', 'cast', 'character', 'production', 'script', 'actor', 'director']</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.6708850893472472</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6629392884877827</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6068501438223768</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5017763141975303</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -676,23 +676,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['game', 'player', 'gameplay', 'games', 'players', 'soundtrack', 'mario', 'playstation', 'graphics', 'mode', 'hero', 'nintendo', 'characters', 'released', 'version']</t>
+          <t>['species', 'shark', 'genus', 'sharks', 'cap', 'fruit', 'stem', 'fungus', 'spores', 'brown', 'nest', 'females', 'habitat', 'eggs', 'fin']</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.7190914950495463</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.6747862659157132</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.6723356661393743</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.6697060257897562</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.6640719527389186</v>
       </c>
     </row>
     <row r="11">
@@ -701,23 +701,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['innings', 'runs', 'league', 'baseball', 'nba', 'batting', 'season', 'career', 'team', 'scored', 'wickets', 'basketball', 'games', 'rebounds', 'batted']</t>
+          <t>['election', 'campaign', 'political', 'party', 'bush', 'government', 'republican', 'vote', 'presidential', 'president', 'labour', 'democratic', 'senate', 'candidate', 'women']</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.8901149788288089</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8710989796136231</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8391870939273561</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8278851306559769</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8240034880070073</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -726,23 +726,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['film', 'films', 'bond', 'disney', 'role', 'movie', 'actor', 'starred', 'cast', 'box', 'tamil', 'director', 'filming', 'grossing', 'production']</t>
+          <t>['episode', 'dwight', 'glee', 'michael', 'jim', 'liz', 'pam', 'nbc', 'viewers', 'andy', 'jack', 'office', 'watched', 'jenna', 'fey']</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.8769949182038974</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.8587329822795781</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.840984288978215</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.8401846814872316</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.8316889610000482</v>
       </c>
     </row>
     <row r="13">
@@ -751,7 +751,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['french', 'british', 'governor', 'militia', 'troops', 'battle', 'massachusetts', 'boston', 'command', 'kentucky', 'fort', 'men', 'army', 'fleet', 'general']</t>
+          <t>['king', 'polish', 'arab', 'son', 'emperor', 'reign', 'pope', 'poland', 'henry', 'hungary', 'royal', 'constantine', 'byzantine', 'bishop', 'died']</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -776,23 +776,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['castle', 'century', 'station', 'church', 'castles', 'built', 'bridge', 'tower', 'pier', 'railway', 'bailey', 'river', 'building', 'trains', 'bristol']</t>
+          <t>['french', 'persian', 'army', 'british', 'battle', 'troops', 'fleet', 'siege', 'militia', 'force', 'men', 'cavalry', 'forces', 'expedition', 'ships']</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.8898604909005957</v>
+        <v>0.7480594885459535</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8868397759459766</v>
+        <v>0.5156736224405625</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8754026800263479</v>
+        <v>0.5027485792061874</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8653366724333088</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.8573847899841381</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -801,23 +801,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['match', 'wrestling', 'championship', 'wwe', 'tag', 'raw', 'ring', 'smackdown', 'defeated', 'heavyweight', 'feud', 'event', 'wwf', 'michaels', 'title']</t>
+          <t>['hitler', 'commander', 'officer', 'war', 'physics', 'command', 'holocaust', 'german', 'promoted', 'nuclear', 'lieutenant', 'jews', 'awarded', 'nazi', 'germany']</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.8994461037061843</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8970629673216594</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8929929559887967</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8918549569086228</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.8901445872411098</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -826,7 +826,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['building', 'city', 'park', 'chicago', 'memorial', 'memorials', 'library', 'fountain', 'indiana', 'square', 'galveston', 'street', 'buildings', 'bay', 'courthouse']</t>
+          <t>['building', 'mosque', 'museum', 'temple', 'pier', 'square', 'chicago', 'park', 'hall', 'library', 'mall', 'memorial', 'buildings', 'memorials', 'floor']</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -851,23 +851,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['simpsons', 'episodes', 'episode', 'homer', 'stan', 'parker', 'kenny', 'animated', 'kyle', 'nickelodeon', 'voice', 'lisa', 'jake', 'television', 'voiced']</t>
+          <t>['castle', 'century', 'church', 'castles', 'scotland', 'tower', 'bailey', 'stone', 'walls', 'scottish', 'built', 'painting', 'chancel', 'wall', 'medieval']</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.8410681958333622</v>
+        <v>0.8937091892958637</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8408707414726451</v>
+        <v>0.8911133937740987</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8342199186176124</v>
+        <v>0.8887153938999705</v>
       </c>
       <c r="F17" t="n">
-        <v>0.789329704457635</v>
+        <v>0.8870449593987323</v>
       </c>
       <c r="G17" t="n">
-        <v>0.7601764068907592</v>
+        <v>0.8721258415930611</v>
       </c>
     </row>
     <row r="18">
@@ -876,23 +876,23 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['battalion', 'brigade', 'division', 'regiment', 'infantry', 'battalions', 'squadron', 'training', 'unit', 'units', 'raaf', 'australian', '2nd', 'japanese', '1st']</t>
+          <t>['creek', 'watershed', 'river', 'dam', 'bridge', 'flows', 'volcano', 'area', 'lake', 'park', 'feet', 'water', 'canal', 'city', 'lava']</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.8976577662524322</v>
+        <v>0.5839065515385909</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8907184988740995</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8847848941949625</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.8843924798218827</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.8779918499766377</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -901,23 +901,23 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['olympics', 'athletes', 'olympic', 'medal', 'meter', 'freestyle', 'championships', 'beijing', 'medals', 'seconds', 'relay', 'gold', 'competed', 'games', 'summer']</t>
+          <t>['battalion', 'brigade', 'division', 'regiment', 'infantry', 'battalions', 'units', 'unit', 'training', 'squadron', '1st', '2nd', 'artillery', 'casualties', 'forces']</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.8995757378356433</v>
+        <v>0.8848648021345178</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8992369611502073</v>
+        <v>0.8839354988419402</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8962133967040117</v>
+        <v>0.8789412214994843</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8959980814952551</v>
+        <v>0.8758305499223621</v>
       </c>
       <c r="G19" t="n">
-        <v>0.8939842142569264</v>
+        <v>0.8662346020319874</v>
       </c>
     </row>
     <row r="20">
@@ -926,23 +926,23 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>['oxford', 'cambridge', 'race', 'boat', 'blues', 'rowed', 'rowing', 'lengths', 'crews', 'rower', 'thames', 'races', 'crew', 'universities', 'umpired']</t>
+          <t>['film', 'tamil', 'telugu', 'chinese', 'india', 'han', 'hindu', 'indian', 'films', 'mumbai', 'hindi', 'china', 'cinema', 'sanskrit', 'bollywood']</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.8933404872102932</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8931113782617631</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.885902464354956</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.8857321694324698</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.8841812799749215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -951,23 +951,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['poem', 'poems', 'poetry', 'poet', 'han', 'shakespeare', 'ode', 'riley', 'text', 'sanskrit', 'texts', 'poetic', 'literary', 'works', 'smart']</t>
+          <t>['station', 'trains', 'railway', 'line', 'locomotives', 'services', 'train', 'locomotive', 'oslo', 'railways', 'passenger', 'platforms', 'tunnel', 'nok', 'platform']</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.7934033862609332</v>
+        <v>0.89870990323392</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7498369472030213</v>
+        <v>0.8983600803874914</v>
       </c>
       <c r="E21" t="n">
-        <v>0.7379377015299917</v>
+        <v>0.897762142582303</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6746928011070878</v>
+        <v>0.8962369114667619</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6746928011070878</v>
+        <v>0.8949127529183183</v>
       </c>
     </row>
     <row r="22">
@@ -976,23 +976,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>['breed', 'horses', 'horse', 'breeds', 'dog', 'dogs', 'stud', 'breeding', 'bred', 'arabian', 'stallion', 'riding', 'breeders', 'pony', 'stakes']</t>
+          <t>['oxford', 'cambridge', 'race', 'boat', 'blues', 'rowed', 'rowing', 'lengths', 'crews', 'rower', 'thames', 'races', 'crew', 'universities', 'umpired']</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.8816342584032073</v>
+        <v>0.8979338632907142</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8789928337046216</v>
+        <v>0.8887903688875138</v>
       </c>
       <c r="E22" t="n">
-        <v>0.8704516537222983</v>
+        <v>0.8882041396098418</v>
       </c>
       <c r="F22" t="n">
-        <v>0.8349591423823824</v>
+        <v>0.882452273810741</v>
       </c>
       <c r="G22" t="n">
-        <v>0.8335245520367489</v>
+        <v>0.8787590406208141</v>
       </c>
     </row>
     <row r="23">
@@ -1001,23 +1001,23 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['creek', 'watershed', 'dam', 'volcano', 'lava', 'pipeline', 'flows', 'volcanic', 'trout', 'mountain', 'park', 'eruption', 'river', 'feet', 'cubic']</t>
+          <t>['aircraft', 'engine', 'flight', 'spacecraft', 'wing', 'fuselage', 'mission', 'fuel', 'engines', 'prototype', 'air', 'nasa', 'radar', 'apollo', 'landing']</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.8962382467061845</v>
+        <v>0.8333601813108831</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8748386294659284</v>
+        <v>0.8057179101303708</v>
       </c>
       <c r="E23" t="n">
-        <v>0.867797248506632</v>
+        <v>0.7985182691352919</v>
       </c>
       <c r="F23" t="n">
-        <v>0.8564198104348976</v>
+        <v>0.7712858339119837</v>
       </c>
       <c r="G23" t="n">
-        <v>0.8476569538688893</v>
+        <v>0.7503973333214373</v>
       </c>
     </row>
     <row r="24">
@@ -1026,23 +1026,23 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>['aircraft', 'engine', 'flight', 'fuselage', 'wing', 'air', 'engines', 'prototype', 'radar', 'fighter', 'fuel', 'raf', 'speed', 'car', 'testing']</t>
+          <t>['breed', 'horses', 'horse', 'breeds', 'dog', 'dogs', 'stud', 'breeding', 'bred', 'arabian', 'stallion', 'breeders', 'riding', 'stakes', 'pony']</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.8923838961112569</v>
+        <v>0.8932864060099441</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8550846709305449</v>
+        <v>0.8908926753823655</v>
       </c>
       <c r="E24" t="n">
-        <v>0.8372260935178961</v>
+        <v>0.8849904267064944</v>
       </c>
       <c r="F24" t="n">
-        <v>0.8259438922902133</v>
+        <v>0.8808473947187662</v>
       </c>
       <c r="G24" t="n">
-        <v>0.8191061185877834</v>
+        <v>0.8770714324977951</v>
       </c>
     </row>
     <row r="25">
@@ -1051,23 +1051,23 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>['trains', 'locomotives', 'locomotive', 'oslo', 'line', 'nok', 'train', 'station', 'tunnel', 'railway', 'class', 'rail', 'railways', 'passenger', 'trondheim']</t>
+          <t>['governor', 'kentucky', 'massachusetts', 'colony', 'boston', 'virginia', 'elected', 'fraternity', 'plymouth', 'davis', 'colonial', 'served', 'legislature', 'confederate', 'state']</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.8999502951522912</v>
+        <v>0.7586971055509638</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8961412141544224</v>
+        <v>0.7473527771497847</v>
       </c>
       <c r="E25" t="n">
-        <v>0.8946205474495311</v>
+        <v>0.7105972173477707</v>
       </c>
       <c r="F25" t="n">
-        <v>0.894024604961298</v>
+        <v>0.6650399700623348</v>
       </c>
       <c r="G25" t="n">
-        <v>0.8928936403254673</v>
+        <v>0.6638155381445657</v>
       </c>
     </row>
     <row r="26">
@@ -1076,23 +1076,23 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>['manga', 'anime', 'comics', 'stories', 'story', 'comic', 'magazine', 'volume', 'volumes', 'fiction', 'gay', 'characters', 'pulp', 'published', 'issue']</t>
+          <t>['lap', 'race', 'drivers', 'laps', 'pit', 'driver', 'car', 'ferrari', 'qualifying', 'prix', 'session', 'fastest', 'ahead', 'hamilton', 'caution']</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.8971397471299966</v>
+        <v>0.8999019745297119</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8950281123517705</v>
+        <v>0.8959473741163052</v>
       </c>
       <c r="E26" t="n">
-        <v>0.887937349280863</v>
+        <v>0.8953780308537146</v>
       </c>
       <c r="F26" t="n">
-        <v>0.8853554957904606</v>
+        <v>0.8931294936122821</v>
       </c>
       <c r="G26" t="n">
-        <v>0.8776313937324671</v>
+        <v>0.8930217583143408</v>
       </c>
     </row>
     <row r="27">
@@ -1101,23 +1101,23 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>['lap', 'race', 'drivers', 'laps', 'pit', 'car', 'driver', 'ferrari', 'qualifying', 'prix', 'session', 'fastest', 'ahead', 'caution', 'hamilton']</t>
+          <t>['poem', 'poems', 'poetry', 'poet', 'shakespeare', 'ode', 'riley', 'smart', 'narrator', 'published', 'poetic', 'stanza', 'literary', 'thomas', 'works']</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.899589057229355</v>
+        <v>0.8733391630688715</v>
       </c>
       <c r="D27" t="n">
-        <v>0.898335132169527</v>
+        <v>0.870793783177932</v>
       </c>
       <c r="E27" t="n">
-        <v>0.8977043810937559</v>
+        <v>0.8670785808638413</v>
       </c>
       <c r="F27" t="n">
-        <v>0.8974674594264279</v>
+        <v>0.8467104875439323</v>
       </c>
       <c r="G27" t="n">
-        <v>0.8950169921998243</v>
+        <v>0.8463444865538601</v>
       </c>
     </row>
     <row r="28">
@@ -1126,23 +1126,23 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>['yard', 'yards', 'touchdown', 'tech', 'alabama', 'bowl', 'quarter', 'michigan', 'offense', 'football', 'pass', 'rushing', 'quarterback', 'conference', 'touchdowns']</t>
+          <t>['match', 'event', 'ring', 'michaels', 'undertaker', 'championship', 'pinfall', 'wrestlers', 'heavyweight', 'tag', 'raw', 'triple', 'wrestling', 'wwe', 'matches']</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.894528845283853</v>
+        <v>0.8994762429384142</v>
       </c>
       <c r="D28" t="n">
-        <v>0.8942743768305161</v>
+        <v>0.8979860590068155</v>
       </c>
       <c r="E28" t="n">
-        <v>0.8915809848785308</v>
+        <v>0.8971165159985877</v>
       </c>
       <c r="F28" t="n">
-        <v>0.8822598376371611</v>
+        <v>0.8963795799168726</v>
       </c>
       <c r="G28" t="n">
-        <v>0.8818717964523473</v>
+        <v>0.8957676768330787</v>
       </c>
     </row>
     <row r="29">
@@ -1151,23 +1151,23 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>['wine', 'chicken', 'cheese', 'bacon', 'recipes', 'sandwich', 'fried', 'dish', 'dishes', 'cuisine', 'ingredients', 'cooking', 'beef', 'food', 'product']</t>
+          <t>['bach', 'text', 'conscience', 'jesus', 'movements', 'movement', 'soprano', 'gospel', 'hebrew', 'aria', 'alto', 'manuscripts', 'leipzig', 'manuscript', 'tenor']</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.8959564721457992</v>
+        <v>0.8975454596516902</v>
       </c>
       <c r="D29" t="n">
-        <v>0.8764875153097185</v>
+        <v>0.8910942345679709</v>
       </c>
       <c r="E29" t="n">
-        <v>0.8751223183597634</v>
+        <v>0.6825373929796601</v>
       </c>
       <c r="F29" t="n">
-        <v>0.8695782306780427</v>
+        <v>0.6647861341660084</v>
       </c>
       <c r="G29" t="n">
-        <v>0.8405835638130674</v>
+        <v>0.62131293257349</v>
       </c>
     </row>
     <row r="30">
@@ -1176,23 +1176,23 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>['persian', 'army', 'byzantine', 'athens', 'greeks', 'greece', 'battle', 'alexander', 'greek', 'siege', 'muslim', 'cavalry', 'byzantines', 'arab', 'ottoman']</t>
+          <t>['wine', 'bacon', 'chicken', 'cheese', 'recipes', 'sandwich', 'fried', 'dish', 'dishes', 'cuisine', 'ingredients', 'cooking', 'beef', 'food', 'meat']</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.8918801717134893</v>
+        <v>0.8730963660933672</v>
       </c>
       <c r="D30" t="n">
-        <v>0.8818350529814225</v>
+        <v>0.8577086701968332</v>
       </c>
       <c r="E30" t="n">
-        <v>0.8652987059208482</v>
+        <v>0.85182141021078</v>
       </c>
       <c r="F30" t="n">
-        <v>0.8382668064278899</v>
+        <v>0.8414287363318577</v>
       </c>
       <c r="G30" t="n">
-        <v>0.8361667774863114</v>
+        <v>0.8364555112195488</v>
       </c>
     </row>
     <row r="31">
@@ -1201,23 +1201,23 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>['bach', 'text', 'movements', 'movement', 'soprano', 'gospel', 'jesus', 'hebrew', 'aria', 'alto', 'manuscripts', 'leipzig', 'tenor', 'hymn', 'matthew']</t>
+          <t>['coaster', 'ride', 'roller', 'riders', 'train', 'coasters', 'flags', 'park', 'lift', 'cedar', 'drop', 'brake', 'trains', 'steel', 'hill']</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.8252006431725999</v>
+        <v>0.8893722263818562</v>
       </c>
       <c r="D31" t="n">
-        <v>0.7995705958719048</v>
+        <v>0.8838690571438658</v>
       </c>
       <c r="E31" t="n">
-        <v>0.7897658468010489</v>
+        <v>0.8830964093708745</v>
       </c>
       <c r="F31" t="n">
-        <v>0.694089658257831</v>
+        <v>0.8818360647032901</v>
       </c>
       <c r="G31" t="n">
-        <v>0.6796103510471005</v>
+        <v>0.8754673687299952</v>
       </c>
     </row>
     <row r="32">
@@ -1226,23 +1226,23 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>['coaster', 'ride', 'roller', 'riders', 'train', 'coasters', 'flags', 'park', 'lift', 'cedar', 'drop', 'brake', 'trains', 'steel', 'hill']</t>
+          <t>['yard', 'yards', 'tech', 'touchdown', 'bowl', 'quarter', 'michigan', 'offense', 'pass', 'conference', 'quarterback', 'rushing', 'ball', 'football', 'coach']</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.8957994125240196</v>
+        <v>0.8968452179658302</v>
       </c>
       <c r="D32" t="n">
-        <v>0.8944680211075516</v>
+        <v>0.8953055986316139</v>
       </c>
       <c r="E32" t="n">
-        <v>0.882740977230002</v>
+        <v>0.8949958707115958</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8788186276840939</v>
+        <v>0.8939864705382187</v>
       </c>
       <c r="G32" t="n">
-        <v>0.8685395620705895</v>
+        <v>0.8887982183247037</v>
       </c>
     </row>
     <row r="33">
@@ -1251,23 +1251,23 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>['formula', 'function', 'matrix', 'linear', 'functions', 'space', 'constant', 'defined', 'language', 'filter', 'frequency', 'mass', 'derivative', 'kilogram', 'units']</t>
+          <t>['athletes', 'olympics', 'olympic', 'beijing', 'heat', 'seconds', 'athlete', 'round', 'games', 'paralympic', 'summer', 'medal', 'medals', 'event', 'events']</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.8809363094291861</v>
+        <v>0.8995165545181665</v>
       </c>
       <c r="D33" t="n">
-        <v>0.8727212074205268</v>
+        <v>0.8985515383783425</v>
       </c>
       <c r="E33" t="n">
-        <v>0.8657413410672804</v>
+        <v>0.8978675362611077</v>
       </c>
       <c r="F33" t="n">
-        <v>0.8410292524168366</v>
+        <v>0.8974710136989418</v>
       </c>
       <c r="G33" t="n">
-        <v>0.8278142687388411</v>
+        <v>0.8971197912971408</v>
       </c>
     </row>
     <row r="34">
@@ -1276,23 +1276,23 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>['amendment', 'constitution', 'singapore', 'law', 'court', 'courts', 'judicial', 'parliament', 'article', 'constitutional', 'justice', 'shall', 'clause', 'act', 'rights']</t>
+          <t>['comics', 'fiction', 'stories', 'gay', 'magazine', 'pulp', 'comic', 'story', 'science', 'lgbt', 'adventures', 'issue', 'cartoonist', 'belgian', 'published']</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.896567062441377</v>
+        <v>0.8927240067664698</v>
       </c>
       <c r="D34" t="n">
-        <v>0.856853908291624</v>
+        <v>0.8911233893797638</v>
       </c>
       <c r="E34" t="n">
-        <v>0.8499817690647762</v>
+        <v>0.8781665436062777</v>
       </c>
       <c r="F34" t="n">
-        <v>0.847849802827159</v>
+        <v>0.8775836288391855</v>
       </c>
       <c r="G34" t="n">
-        <v>0.8393930103432241</v>
+        <v>0.8768399241551521</v>
       </c>
     </row>
     <row r="35">
@@ -1301,23 +1301,23 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>['management', 'twitter', 'investment', 'bank', 'billion', 'equity', 'watson', 'design', 'banking', 'company', 'users', 'firm', 'business', 'merger', 'assets']</t>
+          <t>['formula', 'function', 'matrix', 'linear', 'cylinders', 'constant', 'functions', 'cylinder', 'defined', 'filter', 'frequency', 'voltage', 'gas', 'mass', 'derivative']</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.7552939216034684</v>
+        <v>0.8440333855830487</v>
       </c>
       <c r="D35" t="n">
-        <v>0.7267929555276822</v>
+        <v>0.839820454310136</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6967749222492603</v>
+        <v>0.8350875065268301</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6373313443470506</v>
+        <v>0.7965054795319079</v>
       </c>
       <c r="G35" t="n">
-        <v>0.5127592840712791</v>
+        <v>0.7595619892800839</v>
       </c>
     </row>
     <row r="36">
@@ -1326,23 +1326,23 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>['mosque', 'temple', 'congregation', 'wall', 'palace', 'hall', 'jewish', 'jews', 'shrine', 'tomb', 'temples', 'cave', 'jerusalem', 'christians', 'dome']</t>
+          <t>['management', 'twitter', 'investment', 'bank', 'billion', 'equity', 'design', 'company', 'banking', 'firm', 'users', 'business', 'corporate', 'merger', 'assets']</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.8800210270419596</v>
+        <v>0.8949281676384304</v>
       </c>
       <c r="D36" t="n">
-        <v>0.8603731340226697</v>
+        <v>0.8440217284317534</v>
       </c>
       <c r="E36" t="n">
-        <v>0.8394945352111849</v>
+        <v>0.7797935453407455</v>
       </c>
       <c r="F36" t="n">
-        <v>0.8389417350647215</v>
+        <v>0.711255270275215</v>
       </c>
       <c r="G36" t="n">
-        <v>0.8371138017460441</v>
+        <v>0.6406559182345594</v>
       </c>
     </row>
     <row r="37">
@@ -1351,23 +1351,23 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>['scotland', 'scottish', 'island', 'islands', 'norse', 'century', 'edinburgh', 'isles', 'houses', 'architecture', 'mainland', 'scots', 'glasgow', 'highlands', 'churches']</t>
+          <t>['fischer', 'chess', 'fight', 'tournament', 'round', 'boxing', 'champion', 'hughes', 'bout', 'trinidad', 'robinson', 'punches', 'black', 'knockout', 'unanimous']</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.8927239821043242</v>
+        <v>0.8989686551640569</v>
       </c>
       <c r="D37" t="n">
-        <v>0.8429310496340747</v>
+        <v>0.8920171123110907</v>
       </c>
       <c r="E37" t="n">
-        <v>0.8420592345831623</v>
+        <v>0.8900382144975235</v>
       </c>
       <c r="F37" t="n">
-        <v>0.8257043321464712</v>
+        <v>0.8900382144975235</v>
       </c>
       <c r="G37" t="n">
-        <v>0.8000422618234712</v>
+        <v>0.8707150422517377</v>
       </c>
     </row>
     <row r="38">
@@ -1376,23 +1376,23 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>['croatian', 'yugoslav', 'partisans', 'serbian', 'croatia', 'yugoslavia', 'partisan', 'serbs', 'bosnia', 'belgrade', 'serbia', 'germans', 'civilians', 'division', 'forces']</t>
+          <t>['amendment', 'court', 'constitution', 'clause', 'justices', 'shall', 'rights', 'congress', 'declaration', 'courts', 'law', 'states', 'defendant', 'justice', 'jurisdiction']</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.866186533677501</v>
+        <v>0.89497425173117</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8639887463519905</v>
+        <v>0.8798216214932936</v>
       </c>
       <c r="E38" t="n">
-        <v>0.7779175456682912</v>
+        <v>0.8790731724001271</v>
       </c>
       <c r="F38" t="n">
-        <v>0.7770886357257731</v>
+        <v>0.8740579863359603</v>
       </c>
       <c r="G38" t="n">
-        <v>0.7506051997966334</v>
+        <v>0.8445541015600149</v>
       </c>
     </row>
     <row r="39">
@@ -1401,23 +1401,23 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>['plants', 'plant', 'botanical', 'tree', 'camouflage', 'animals', 'organisms', 'animal', 'gardens', 'species', 'garden', 'tea', 'trees', 'ecology', 'predators']</t>
+          <t>['plants', 'plant', 'botanical', 'camouflage', 'animals', 'gardens', 'animal', 'garden', 'tea', 'species', 'predators', 'coloration', 'predator', 'organisms', 'mimic']</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.8451232096314275</v>
+        <v>0.8659271849951133</v>
       </c>
       <c r="D39" t="n">
-        <v>0.815992496019847</v>
+        <v>0.8582529653349864</v>
       </c>
       <c r="E39" t="n">
-        <v>0.8104518133702522</v>
+        <v>0.8576701135121109</v>
       </c>
       <c r="F39" t="n">
-        <v>0.7960936971394411</v>
+        <v>0.8502484348111302</v>
       </c>
       <c r="G39" t="n">
-        <v>0.7602634450909223</v>
+        <v>0.8468069059304454</v>
       </c>
     </row>
     <row r="40">
@@ -1426,23 +1426,23 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>['phillies', 'inning', 'yankees', 'dodgers', 'teams', 'breaker', 'giants', 'mlb', 'tie', 'yankee', 'postseason', 'game', 'run', 'pitcher', 'baseball']</t>
+          <t>['phillies', 'inning', 'yankees', 'dodgers', 'teams', 'breaker', 'giants', 'mlb', 'tie', 'yankee', 'postseason', 'game', 'run', 'pitcher', 'innings']</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.8994062182118583</v>
+        <v>0.8980414856431461</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8977955928166224</v>
+        <v>0.8979293502517113</v>
       </c>
       <c r="E40" t="n">
-        <v>0.8945722923500797</v>
+        <v>0.8971451357004047</v>
       </c>
       <c r="F40" t="n">
-        <v>0.8936233587903845</v>
+        <v>0.8958870986955263</v>
       </c>
       <c r="G40" t="n">
-        <v>0.8931667805655698</v>
+        <v>0.8957411228909988</v>
       </c>
     </row>
     <row r="41">
@@ -1451,23 +1451,23 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>['painting', 'paintings', 'art', 'artist', 'serbian', 'works', 'marie', 'exhibition', 'copenhagen', 'photography', 'photographers', 'canvas', 'painted', 'symphony', 'portrait']</t>
+          <t>['bond', 'film', 'casino', 'agent', 'films', 'kill', 'sequence', 'filming', 'majesty', 'secret', 'licence', 'spy', 'scenes', 'villain', 'chase']</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.8986584859247188</v>
+        <v>0.8910979414173759</v>
       </c>
       <c r="D41" t="n">
-        <v>0.895602751561582</v>
+        <v>0.8750005047659206</v>
       </c>
       <c r="E41" t="n">
-        <v>0.8872227294448619</v>
+        <v>0.8726755074069061</v>
       </c>
       <c r="F41" t="n">
-        <v>0.8811933738725986</v>
+        <v>0.8683127304238655</v>
       </c>
       <c r="G41" t="n">
-        <v>0.8690559314362738</v>
+        <v>0.8506412338159358</v>
       </c>
     </row>
     <row r="42">
@@ -1476,23 +1476,23 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>['spacecraft', 'apollo', 'nasa', 'orbit', 'mission', 'lunar', 'launch', 'saturn', 'docking', 'flight', 'manned', 'module', 'space', 'landing', 'earth']</t>
+          <t>['baptism', 'congregation', 'christ', 'churches', 'church', 'spirit', 'congregations', 'holy', 'assemblies', 'god', 'worship', 'jewish', 'faith', 'israel', 'christian']</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.8693634243960719</v>
+        <v>0.8948106782643783</v>
       </c>
       <c r="D42" t="n">
-        <v>0.8639757808198418</v>
+        <v>0.8789385891348759</v>
       </c>
       <c r="E42" t="n">
-        <v>0.8611228103650478</v>
+        <v>0.8704072773165948</v>
       </c>
       <c r="F42" t="n">
-        <v>0.8599091447790976</v>
+        <v>0.8574424715688219</v>
       </c>
       <c r="G42" t="n">
-        <v>0.8569662011247938</v>
+        <v>0.8541920333177899</v>
       </c>
     </row>
     <row r="43">
@@ -1501,23 +1501,23 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>['contest', 'broadcaster', 'semi', 'countries', 'jury', 'final', 'participating', 'greece', 'voting', 'host', 'idol', 'entry', 'philippine', 'song', 'country']</t>
+          <t>['painting', 'paintings', 'symphony', 'art', 'works', 'swan', 'white', 'abstract', 'artist', 'canvas', 'dots', 'girl', 'prelude', 'okay', 'work']</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.8977674172528227</v>
+        <v>0.8906945911237063</v>
       </c>
       <c r="D43" t="n">
-        <v>0.897027332936389</v>
+        <v>0.8872971731033414</v>
       </c>
       <c r="E43" t="n">
-        <v>0.8914754394199775</v>
+        <v>0.8838494513808206</v>
       </c>
       <c r="F43" t="n">
-        <v>0.8882109899629327</v>
+        <v>0.8833219142057193</v>
       </c>
       <c r="G43" t="n">
-        <v>0.8860614465100162</v>
+        <v>0.8823050276442443</v>
       </c>
     </row>
     <row r="44">
@@ -1526,23 +1526,23 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>['lighthouse', 'light', 'keeper', 'tower', 'lens', 'keepers', 'concrete', 'connecticut', 'lamp', 'cottages', 'installed', 'constructed', 'lamps', 'island', 'iron']</t>
+          <t>['contest', 'broadcaster', 'semi', 'countries', 'jury', 'final', 'participating', 'greece', 'voting', 'host', 'idol', 'entry', 'philippine', 'song', 'country']</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.8892793712174863</v>
+        <v>0.8988321755029557</v>
       </c>
       <c r="D44" t="n">
-        <v>0.8758949069477608</v>
+        <v>0.8913088929608021</v>
       </c>
       <c r="E44" t="n">
-        <v>0.8724615980009904</v>
+        <v>0.8901373609831699</v>
       </c>
       <c r="F44" t="n">
-        <v>0.865858147221465</v>
+        <v>0.8860665469551351</v>
       </c>
       <c r="G44" t="n">
-        <v>0.8555457530311984</v>
+        <v>0.8851769075878799</v>
       </c>
     </row>
     <row r="45">
@@ -1551,23 +1551,23 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>['ben', 'survivors', 'shannon', 'island', 'freighter', 'charlotte', 'bernard', 'michael', 'plane', 'daniel', 'tom', 'frank', 'dave', 'kate', 'oceanic']</t>
+          <t>['motorway', 'croatia', 'adriatic', 'croatian', 'toll', 'traffic', 'interchanges', 'kilometre', 'route', 'interchange', 'kilometres', 'section', 'areas', 'rest', 'yugoslavia']</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.8843045125965368</v>
+        <v>0.8996915588273637</v>
       </c>
       <c r="D45" t="n">
-        <v>0.8697161586874406</v>
+        <v>0.8987440332007089</v>
       </c>
       <c r="E45" t="n">
-        <v>0.8588155624058443</v>
+        <v>0.8985750018981516</v>
       </c>
       <c r="F45" t="n">
-        <v>0.842997492066711</v>
+        <v>0.8967267806973311</v>
       </c>
       <c r="G45" t="n">
-        <v>0.8361383388954475</v>
+        <v>0.8948623087482174</v>
       </c>
     </row>
     <row r="46">
@@ -1576,23 +1576,23 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>['motorway', 'croatia', 'adriatic', 'croatian', 'toll', 'traffic', 'interchanges', 'kilometre', 'route', 'interchange', 'kilometres', 'section', 'areas', 'rest', 'yugoslavia']</t>
+          <t>['singapore', 'law', 'judicial', 'constitution', 'parliament', 'article', 'courts', 'minister', 'court', 'constitutional', 'detention', 'persons', 'public', 'act', 'mps']</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.8974268013124268</v>
+        <v>0.8770626811049285</v>
       </c>
       <c r="D46" t="n">
-        <v>0.8937423833377387</v>
+        <v>0.8585608510420158</v>
       </c>
       <c r="E46" t="n">
-        <v>0.8931426754495102</v>
+        <v>0.843812884670976</v>
       </c>
       <c r="F46" t="n">
-        <v>0.8849775354748642</v>
+        <v>0.8348986712852453</v>
       </c>
       <c r="G46" t="n">
-        <v>0.8681855529047939</v>
+        <v>0.8346817191588695</v>
       </c>
     </row>
     <row r="47">
@@ -1601,23 +1601,23 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>['rockets', 'nba', 'arena', 'playoffs', 'houston', 'team', 'franchise', 'ownership', 'finals', 'relocation', 'toronto', 'draft', 'games', 'pick', 'season']</t>
+          <t>['lighthouse', 'light', 'keeper', 'tower', 'lens', 'keepers', 'concrete', 'lamp', 'cottages', 'constructed', 'lamps', 'connecticut', 'installed', 'iron', 'restoration']</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.8994844352280338</v>
+        <v>0.8901361650547728</v>
       </c>
       <c r="D47" t="n">
-        <v>0.8965042202987602</v>
+        <v>0.8836495611537444</v>
       </c>
       <c r="E47" t="n">
-        <v>0.8829335302376713</v>
+        <v>0.8765805697707494</v>
       </c>
       <c r="F47" t="n">
-        <v>0.8826075439356167</v>
+        <v>0.8727539804239123</v>
       </c>
       <c r="G47" t="n">
-        <v>0.8796285845221472</v>
+        <v>0.8725949734416462</v>
       </c>
     </row>
     <row r="48">
@@ -1633,16 +1633,16 @@
         <v>0.8996513236405467</v>
       </c>
       <c r="D48" t="n">
-        <v>0.8995021322793546</v>
+        <v>0.8946537850381572</v>
       </c>
       <c r="E48" t="n">
-        <v>0.8878878148021422</v>
+        <v>0.887782942541842</v>
       </c>
       <c r="F48" t="n">
-        <v>0.850146904005964</v>
+        <v>0.874292615387922</v>
       </c>
       <c r="G48" t="n">
-        <v>0.8500225861510472</v>
+        <v>0.8531864252174087</v>
       </c>
     </row>
     <row r="49">
@@ -1651,23 +1651,23 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>['grammy', 'neo', 'hawaiian', 'soul', 'nominees', 'category', 'awards', 'rap', 'award', 'presented', 'categories', 'artists', 'recipients', 'academy', 'disco']</t>
+          <t>['euro', 'coins', 'currency', 'note', 'notes', 'denominations', 'dollar', 'value', 'stripe', 'tender', 'silver', 'thread', 'ink', 'issued', 'signature']</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.899989502367133</v>
+        <v>0.8983674232344895</v>
       </c>
       <c r="D49" t="n">
-        <v>0.899732008444733</v>
+        <v>0.8959558957675202</v>
       </c>
       <c r="E49" t="n">
-        <v>0.8992924662338843</v>
+        <v>0.8894251863981077</v>
       </c>
       <c r="F49" t="n">
-        <v>0.8990640910243387</v>
+        <v>0.8640160310875664</v>
       </c>
       <c r="G49" t="n">
-        <v>0.8987665966169236</v>
+        <v>0.852422230350493</v>
       </c>
     </row>
     <row r="50">
@@ -1676,23 +1676,23 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>['euro', 'coins', 'currency', 'note', 'notes', 'denominations', 'dollar', 'value', 'stripe', 'tender', 'silver', 'thread', 'ink', 'issued', 'signature']</t>
+          <t>['grammy', 'hawaiian', 'nominees', 'category', 'awards', 'rap', 'award', 'presented', 'categories', 'recipients', 'academy', 'disco', 'honor', 'proficiency', 'best']</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.8772465903637001</v>
+        <v>0.8993928050554608</v>
       </c>
       <c r="D50" t="n">
-        <v>0.8701030949011572</v>
+        <v>0.8993773076023089</v>
       </c>
       <c r="E50" t="n">
-        <v>0.864386230131906</v>
+        <v>0.8993089570238236</v>
       </c>
       <c r="F50" t="n">
-        <v>0.8626395032219362</v>
+        <v>0.8990830760870018</v>
       </c>
       <c r="G50" t="n">
-        <v>0.8521718393378128</v>
+        <v>0.8990628755699399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>